<commit_message>
Final docs & examples
</commit_message>
<xml_diff>
--- a/source/poiskpostav_OUTPUT.xlsx
+++ b/source/poiskpostav_OUTPUT.xlsx
@@ -498,7 +498,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AI14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -875,385 +875,381 @@
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
         <is>
-          <t>2.03</t>
+          <t>2.06</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>autoopt.ru</t>
+          <t>rezina74.ru</t>
         </is>
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Авто-Альянс, ООО</t>
+          <t>Челябрезинатехника, ООО</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "АВТО-АЛЬЯНС"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ЧЕЛЯБРЕЗИНАТЕХНИКА"</t>
         </is>
       </c>
       <c r="E5" s="7" t="inlineStr">
         <is>
-          <t>г. Москва, ул. Большая Почтовая, д. 26В, стр. 1, КОМ. 502-1</t>
+          <t>г. Челябинск, Троицкий тракт, д. 27Д</t>
         </is>
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
-          <t>8 (800) 555-08-77</t>
+          <t>8 (351) 262-13-57</t>
         </is>
       </c>
       <c r="G5" s="7" t="inlineStr">
         <is>
-          <t>elmiraif@autoopt.ru</t>
+          <t>ofis@rezina74.ru</t>
         </is>
       </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>27.09.2005</t>
+          <t>14.05.2003</t>
         </is>
       </c>
       <c r="I5" s="7" t="inlineStr">
         <is>
-          <t>7720535919</t>
+          <t>7451194400</t>
         </is>
       </c>
       <c r="J5" s="7" t="inlineStr">
         <is>
-          <t>770101001</t>
+          <t>745101001</t>
         </is>
       </c>
       <c r="K5" s="7" t="inlineStr">
         <is>
-          <t>1057748380502</t>
+          <t>1037402903658</t>
         </is>
       </c>
       <c r="L5" s="7" t="inlineStr">
         <is>
-          <t>78399368</t>
+          <t>14838184</t>
         </is>
       </c>
       <c r="M5" s="7" t="inlineStr">
         <is>
-          <t>Найда Евгений Николаевич</t>
+          <t>Логинова Наталья Сергеевна</t>
         </is>
       </c>
       <c r="N5" s="7" t="inlineStr">
         <is>
-          <t>5.5 млрд ₽</t>
+          <t>153.5 млн ₽</t>
         </is>
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>33.4 млн ₽</t>
+          <t>7 млн ₽</t>
         </is>
       </c>
       <c r="P5" s="7" t="inlineStr">
         <is>
-          <t>59%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="Q5" s="7" t="inlineStr">
         <is>
-          <t>1%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="R5" s="7" t="inlineStr">
         <is>
-          <t>40%</t>
-        </is>
-      </c>
-      <c r="S5" s="7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="T5" s="7" t="inlineStr">
-        <is>
-          <t>20%</t>
-        </is>
-      </c>
-      <c r="U5" s="7" t="inlineStr">
-        <is>
-          <t>80%</t>
-        </is>
-      </c>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="S5" s="7" t="inlineStr"/>
+      <c r="T5" s="7" t="inlineStr"/>
+      <c r="U5" s="7" t="inlineStr"/>
       <c r="V5" s="7" t="inlineStr">
         <is>
-          <t>40 тыс ₽</t>
+          <t>10 тыс ₽</t>
         </is>
       </c>
       <c r="W5" s="7" t="inlineStr">
         <is>
-          <t>552.4 млн ₽</t>
+          <t>41.9 млн ₽</t>
         </is>
       </c>
       <c r="X5" s="7" t="inlineStr">
         <is>
-          <t>424</t>
+          <t>188</t>
         </is>
       </c>
       <c r="Y5" s="7" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>102</t>
         </is>
       </c>
       <c r="Z5" s="7" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>16</t>
         </is>
       </c>
       <c r="AA5" s="7" t="inlineStr">
         <is>
-          <t>+ 86</t>
+          <t>+ 87</t>
         </is>
       </c>
       <c r="AB5" s="7" t="inlineStr">
         <is>
-          <t>- 7.4</t>
+          <t>- 0.2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>2.03</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>appnn.ru</t>
+          <t>autoopt.ru</t>
         </is>
       </c>
       <c r="C6" s="7" t="inlineStr">
         <is>
-          <t>Агропромподшипник, ООО</t>
+          <t>Авто-Альянс, ООО</t>
         </is>
       </c>
       <c r="D6" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "АГРОПРОМПОДШИПНИК"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "АВТО-АЛЬЯНС"</t>
         </is>
       </c>
       <c r="E6" s="7" t="inlineStr">
         <is>
-          <t>Нижегородская обл., г.о ГОРОД НИЖНИЙ НОВГОРОД, г НИЖНИЙ НОВГОРОД, ул ГОРДЕЕВСКАЯ, д. 61А, ПОМЕЩ. 5</t>
+          <t>г. Москва, ул. Большая Почтовая, д. 26В, стр. 1, КОМ. 502-1</t>
         </is>
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
-          <t>8 (831) 218-03-10</t>
+          <t>8 (800) 555-08-77</t>
         </is>
       </c>
       <c r="G6" s="7" t="inlineStr">
         <is>
-          <t>agropd@kis.ru</t>
+          <t>elmiraif@autoopt.ru</t>
         </is>
       </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>04.11.1998</t>
+          <t>27.09.2005</t>
         </is>
       </c>
       <c r="I6" s="7" t="inlineStr">
         <is>
-          <t>5258030930</t>
+          <t>7720535919</t>
         </is>
       </c>
       <c r="J6" s="7" t="inlineStr">
         <is>
-          <t>525701001</t>
+          <t>770101001</t>
         </is>
       </c>
       <c r="K6" s="7" t="inlineStr">
         <is>
-          <t>1025202610531</t>
+          <t>1057748380502</t>
         </is>
       </c>
       <c r="L6" s="7" t="inlineStr">
         <is>
-          <t>50331452</t>
+          <t>78399368</t>
         </is>
       </c>
       <c r="M6" s="7" t="inlineStr">
         <is>
-          <t>Рубаха Галина Александровна</t>
+          <t>Найда Евгений Николаевич</t>
         </is>
       </c>
       <c r="N6" s="7" t="inlineStr">
         <is>
-          <t>87.2 млн ₽</t>
+          <t>5.5 млрд ₽</t>
         </is>
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
-          <t>5.3 млн ₽</t>
+          <t>33.4 млн ₽</t>
         </is>
       </c>
       <c r="P6" s="7" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="Q6" s="7" t="inlineStr">
         <is>
+          <t>1%</t>
+        </is>
+      </c>
+      <c r="R6" s="7" t="inlineStr">
+        <is>
+          <t>40%</t>
+        </is>
+      </c>
+      <c r="S6" s="7" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="T6" s="7" t="inlineStr">
+        <is>
           <t>20%</t>
         </is>
       </c>
-      <c r="R6" s="7" t="inlineStr">
-        <is>
-          <t>20%</t>
-        </is>
-      </c>
-      <c r="S6" s="7" t="inlineStr">
-        <is>
-          <t>50%</t>
-        </is>
-      </c>
-      <c r="T6" s="7" t="inlineStr">
-        <is>
-          <t>50%</t>
-        </is>
-      </c>
       <c r="U6" s="7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="V6" s="7" t="inlineStr">
         <is>
-          <t>10 тыс ₽</t>
+          <t>40 тыс ₽</t>
         </is>
       </c>
       <c r="W6" s="7" t="inlineStr">
         <is>
-          <t>26.3 млн ₽</t>
+          <t>552.4 млн ₽</t>
         </is>
       </c>
       <c r="X6" s="7" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>424</t>
         </is>
       </c>
       <c r="Y6" s="7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>157</t>
         </is>
       </c>
       <c r="Z6" s="7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>144</t>
         </is>
       </c>
       <c r="AA6" s="7" t="inlineStr">
         <is>
-          <t>+ 81</t>
-        </is>
-      </c>
-      <c r="AB6" s="7" t="inlineStr"/>
+          <t>+ 86</t>
+        </is>
+      </c>
+      <c r="AB6" s="7" t="inlineStr">
+        <is>
+          <t>- 7.4</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
         <is>
-          <t>1.85</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>autopiter.ru</t>
+          <t>appnn.ru</t>
         </is>
       </c>
       <c r="C7" s="7" t="inlineStr">
         <is>
-          <t>Автопитер.РУ, ООО</t>
+          <t>Агропромподшипник, ООО</t>
         </is>
       </c>
       <c r="D7" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "АВТОПИТЕР.РУ"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "АГРОПРОМПОДШИПНИК"</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
         <is>
-          <t>г. Санкт-Петербург, п. Шушары, Новгородский пр-кт, д. 26, к. 3, стр. 1, ПОМЕЩ. 214</t>
-        </is>
-      </c>
-      <c r="F7" s="7" t="inlineStr"/>
+          <t>Нижегородская обл., г.о ГОРОД НИЖНИЙ НОВГОРОД, г НИЖНИЙ НОВГОРОД, ул ГОРДЕЕВСКАЯ, д. 61А, ПОМЕЩ. 5</t>
+        </is>
+      </c>
+      <c r="F7" s="7" t="inlineStr">
+        <is>
+          <t>8 (831) 218-03-10</t>
+        </is>
+      </c>
       <c r="G7" s="7" t="inlineStr">
         <is>
-          <t>buh@autopiter.ru</t>
+          <t>agropd@kis.ru</t>
         </is>
       </c>
       <c r="H7" s="7" t="inlineStr">
         <is>
-          <t>10.09.2015</t>
+          <t>04.11.1998</t>
         </is>
       </c>
       <c r="I7" s="7" t="inlineStr">
         <is>
-          <t>7820045594</t>
+          <t>5258030930</t>
         </is>
       </c>
       <c r="J7" s="7" t="inlineStr">
         <is>
-          <t>782001001</t>
+          <t>525701001</t>
         </is>
       </c>
       <c r="K7" s="7" t="inlineStr">
         <is>
-          <t>1157847308002</t>
+          <t>1025202610531</t>
         </is>
       </c>
       <c r="L7" s="7" t="inlineStr">
         <is>
-          <t>23170555</t>
+          <t>50331452</t>
         </is>
       </c>
       <c r="M7" s="7" t="inlineStr">
         <is>
-          <t>Заславский Аркадий Леонидович</t>
+          <t>Рубаха Галина Александровна</t>
         </is>
       </c>
       <c r="N7" s="7" t="inlineStr">
         <is>
-          <t>74.7 млн ₽</t>
+          <t>87.2 млн ₽</t>
         </is>
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
-          <t>55.3 млн ₽</t>
+          <t>5.3 млн ₽</t>
         </is>
       </c>
       <c r="P7" s="7" t="inlineStr">
         <is>
+          <t>60%</t>
+        </is>
+      </c>
+      <c r="Q7" s="7" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="R7" s="7" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="S7" s="7" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="T7" s="7" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="U7" s="7" t="inlineStr">
+        <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="Q7" s="7" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="R7" s="7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="S7" s="7" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
-      </c>
-      <c r="T7" s="7" t="inlineStr">
-        <is>
-          <t>50%</t>
-        </is>
-      </c>
-      <c r="U7" s="7" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
-      </c>
       <c r="V7" s="7" t="inlineStr">
         <is>
           <t>10 тыс ₽</t>
@@ -1261,15 +1257,27 @@
       </c>
       <c r="W7" s="7" t="inlineStr">
         <is>
-          <t>192.4 млн ₽</t>
-        </is>
-      </c>
-      <c r="X7" s="7" t="inlineStr"/>
-      <c r="Y7" s="7" t="inlineStr"/>
-      <c r="Z7" s="7" t="inlineStr"/>
+          <t>26.3 млн ₽</t>
+        </is>
+      </c>
+      <c r="X7" s="7" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="Y7" s="7" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="Z7" s="7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="AA7" s="7" t="inlineStr">
         <is>
-          <t>+ 85</t>
+          <t>+ 81</t>
         </is>
       </c>
       <c r="AB7" s="7" t="inlineStr"/>
@@ -1277,99 +1285,103 @@
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
         <is>
-          <t>1.84</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>sibkraspolimer.ru</t>
+          <t>autopiter.ru</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr">
         <is>
-          <t>СК-Полимеры, ООО</t>
+          <t>Автопитер.РУ, ООО</t>
         </is>
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "СК-ПОЛИМЕРЫ"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "АВТОПИТЕР.РУ"</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>Красноярский край, пгт. Березовка, ул. Солнечная, д. 1А</t>
+          <t>г. Санкт-Петербург, п. Шушары, Новгородский пр-кт, д. 26, к. 3, стр. 1, ПОМЕЩ. 214</t>
         </is>
       </c>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
+      <c r="G8" s="7" t="inlineStr">
+        <is>
+          <t>buh@autopiter.ru</t>
+        </is>
+      </c>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>11.12.2008</t>
+          <t>10.09.2015</t>
         </is>
       </c>
       <c r="I8" s="7" t="inlineStr">
         <is>
-          <t>2404012397</t>
+          <t>7820045594</t>
         </is>
       </c>
       <c r="J8" s="7" t="inlineStr">
         <is>
-          <t>240401001</t>
+          <t>782001001</t>
         </is>
       </c>
       <c r="K8" s="7" t="inlineStr">
         <is>
-          <t>1082404001790</t>
+          <t>1157847308002</t>
         </is>
       </c>
       <c r="L8" s="7" t="inlineStr">
         <is>
-          <t>88668243</t>
+          <t>23170555</t>
         </is>
       </c>
       <c r="M8" s="7" t="inlineStr">
         <is>
-          <t>Еремеев Роман Николаевич</t>
+          <t>Заславский Аркадий Леонидович</t>
         </is>
       </c>
       <c r="N8" s="7" t="inlineStr">
         <is>
-          <t>197.3 млн ₽</t>
+          <t>74.7 млн ₽</t>
         </is>
       </c>
       <c r="O8" s="7" t="inlineStr">
         <is>
-          <t>6.5 млн ₽</t>
+          <t>55.3 млн ₽</t>
         </is>
       </c>
       <c r="P8" s="7" t="inlineStr">
         <is>
-          <t>38%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="Q8" s="7" t="inlineStr">
         <is>
-          <t>34%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="R8" s="7" t="inlineStr">
         <is>
-          <t>28%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="S8" s="7" t="inlineStr">
         <is>
-          <t>8%</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="T8" s="7" t="inlineStr">
         <is>
-          <t>33%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="U8" s="7" t="inlineStr">
         <is>
-          <t>59%</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="V8" s="7" t="inlineStr">
@@ -1379,27 +1391,15 @@
       </c>
       <c r="W8" s="7" t="inlineStr">
         <is>
-          <t>103.6 млн ₽</t>
-        </is>
-      </c>
-      <c r="X8" s="7" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="Y8" s="7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Z8" s="7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>192.4 млн ₽</t>
+        </is>
+      </c>
+      <c r="X8" s="7" t="inlineStr"/>
+      <c r="Y8" s="7" t="inlineStr"/>
+      <c r="Z8" s="7" t="inlineStr"/>
       <c r="AA8" s="7" t="inlineStr">
         <is>
-          <t>+ 80</t>
+          <t>+ 85</t>
         </is>
       </c>
       <c r="AB8" s="7" t="inlineStr"/>
@@ -1407,97 +1407,89 @@
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
         <is>
-          <t>1.69</t>
+          <t>1.84</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>din76.ru</t>
+          <t>sibkraspolimer.ru</t>
         </is>
       </c>
       <c r="C9" s="7" t="inlineStr">
         <is>
-          <t>Динамика 76, ООО</t>
+          <t>СК-Полимеры, ООО</t>
         </is>
       </c>
       <c r="D9" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ДИНАМИКА 76"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "СК-ПОЛИМЕРЫ"</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr">
         <is>
-          <t>Ярославская обл., г.о. город Ярославль, г. Ярославль, Ленинградский пр-кт, Д. 33, ПОМЕЩ. 3</t>
-        </is>
-      </c>
-      <c r="F9" s="7" t="inlineStr">
-        <is>
-          <t>8 (4852) 66-01-51</t>
-        </is>
-      </c>
-      <c r="G9" s="7" t="inlineStr">
-        <is>
-          <t>dinamika76-buh@mail.ru</t>
-        </is>
-      </c>
+          <t>Красноярский край, пгт. Березовка, ул. Солнечная, д. 1А</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr">
         <is>
-          <t>10.04.2014</t>
+          <t>11.12.2008</t>
         </is>
       </c>
       <c r="I9" s="7" t="inlineStr">
         <is>
-          <t>7602106039</t>
+          <t>2404012397</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr">
         <is>
-          <t>760201001</t>
+          <t>240401001</t>
         </is>
       </c>
       <c r="K9" s="7" t="inlineStr">
         <is>
-          <t>1147602003097</t>
+          <t>1082404001790</t>
         </is>
       </c>
       <c r="L9" s="7" t="inlineStr">
         <is>
-          <t>33447213</t>
+          <t>88668243</t>
         </is>
       </c>
       <c r="M9" s="7" t="inlineStr">
         <is>
-          <t>Пикин Виктор Александрович</t>
+          <t>Еремеев Роман Николаевич</t>
         </is>
       </c>
       <c r="N9" s="7" t="inlineStr">
         <is>
-          <t>209.7 млн ₽</t>
+          <t>197.3 млн ₽</t>
         </is>
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
-          <t>450 тыс ₽</t>
+          <t>6.5 млн ₽</t>
         </is>
       </c>
       <c r="P9" s="7" t="inlineStr">
         <is>
-          <t>35%</t>
+          <t>38%</t>
         </is>
       </c>
       <c r="Q9" s="7" t="inlineStr">
         <is>
-          <t>3%</t>
+          <t>34%</t>
         </is>
       </c>
       <c r="R9" s="7" t="inlineStr">
         <is>
-          <t>62%</t>
+          <t>28%</t>
         </is>
       </c>
       <c r="S9" s="7" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>8%</t>
         </is>
       </c>
       <c r="T9" s="7" t="inlineStr">
@@ -1507,298 +1499,318 @@
       </c>
       <c r="U9" s="7" t="inlineStr">
         <is>
-          <t>17%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="V9" s="7" t="inlineStr">
         <is>
-          <t>300 тыс ₽</t>
+          <t>10 тыс ₽</t>
         </is>
       </c>
       <c r="W9" s="7" t="inlineStr">
         <is>
-          <t>20.6 млн ₽</t>
+          <t>103.6 млн ₽</t>
         </is>
       </c>
       <c r="X9" s="7" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>7</t>
         </is>
       </c>
       <c r="Y9" s="7" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Z9" s="7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AA9" s="7" t="inlineStr">
         <is>
-          <t>+ 76</t>
-        </is>
-      </c>
-      <c r="AB9" s="7" t="inlineStr">
-        <is>
-          <t>- 8.6</t>
-        </is>
-      </c>
+          <t>+ 80</t>
+        </is>
+      </c>
+      <c r="AB9" s="7" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
         <is>
-          <t>1.68</t>
+          <t>1.69</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>diselars.ru</t>
+          <t>din76.ru</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr">
         <is>
-          <t>ПКФ "Дизель-Арсенал", ООО</t>
+          <t>Динамика 76, ООО</t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ПРОИЗВОДСТВЕННО-КОММЕРЧЕСКАЯ ФИРМА "ДИЗЕЛЬ-АРСЕНАЛ"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ДИНАМИКА 76"</t>
         </is>
       </c>
       <c r="E10" s="7" t="inlineStr">
         <is>
-          <t>г. Ярославль, ул. Угличская, д. 39В, ОФИС 201</t>
+          <t>Ярославская обл., г.о. город Ярославль, г. Ярославль, Ленинградский пр-кт, Д. 33, ПОМЕЩ. 3</t>
         </is>
       </c>
       <c r="F10" s="7" t="inlineStr">
         <is>
-          <t>8 (4852) 59-99-95</t>
-        </is>
-      </c>
-      <c r="G10" s="7" t="inlineStr"/>
+          <t>8 (4852) 66-01-51</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>dinamika76-buh@mail.ru</t>
+        </is>
+      </c>
       <c r="H10" s="7" t="inlineStr">
         <is>
-          <t>28.09.2015</t>
+          <t>10.04.2014</t>
         </is>
       </c>
       <c r="I10" s="7" t="inlineStr">
         <is>
-          <t>7604286161</t>
+          <t>7602106039</t>
         </is>
       </c>
       <c r="J10" s="7" t="inlineStr">
         <is>
-          <t>760401001</t>
+          <t>760201001</t>
         </is>
       </c>
       <c r="K10" s="7" t="inlineStr">
         <is>
-          <t>1157627021771</t>
+          <t>1147602003097</t>
         </is>
       </c>
       <c r="L10" s="7" t="inlineStr">
         <is>
-          <t>57758283</t>
+          <t>33447213</t>
         </is>
       </c>
       <c r="M10" s="7" t="inlineStr">
         <is>
-          <t>Головин Дмитрий Юрьевич</t>
+          <t>Пикин Виктор Александрович</t>
         </is>
       </c>
       <c r="N10" s="7" t="inlineStr">
         <is>
-          <t>488.2 млн ₽</t>
+          <t>209.7 млн ₽</t>
         </is>
       </c>
       <c r="O10" s="7" t="inlineStr">
         <is>
-          <t>604 тыс ₽</t>
+          <t>450 тыс ₽</t>
         </is>
       </c>
       <c r="P10" s="7" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>35%</t>
         </is>
       </c>
       <c r="Q10" s="7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>3%</t>
         </is>
       </c>
       <c r="R10" s="7" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="S10" s="7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>50%</t>
         </is>
       </c>
       <c r="T10" s="7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>33%</t>
         </is>
       </c>
       <c r="U10" s="7" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>17%</t>
         </is>
       </c>
       <c r="V10" s="7" t="inlineStr">
         <is>
-          <t>1 млн ₽</t>
+          <t>300 тыс ₽</t>
         </is>
       </c>
       <c r="W10" s="7" t="inlineStr">
         <is>
-          <t>22.8 млн ₽</t>
+          <t>20.6 млн ₽</t>
         </is>
       </c>
       <c r="X10" s="7" t="inlineStr">
         <is>
+          <t>114</t>
+        </is>
+      </c>
+      <c r="Y10" s="7" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="Z10" s="7" t="inlineStr">
+        <is>
           <t>14</t>
         </is>
       </c>
-      <c r="Y10" s="7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="Z10" s="7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="AA10" s="7" t="inlineStr">
         <is>
-          <t>+ 75</t>
+          <t>+ 76</t>
         </is>
       </c>
       <c r="AB10" s="7" t="inlineStr">
         <is>
-          <t>- 7.6</t>
+          <t>- 8.6</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="inlineStr">
         <is>
-          <t>1.56</t>
+          <t>1.68</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>rti-altai.ru</t>
+          <t>diselars.ru</t>
         </is>
       </c>
       <c r="C11" s="7" t="inlineStr">
         <is>
-          <t>Резинотехника-Алтай, ООО</t>
+          <t>ПКФ "Дизель-Арсенал", ООО</t>
         </is>
       </c>
       <c r="D11" s="7" t="inlineStr">
         <is>
-          <t>Общество с ограниченной ответственностью "РЕЗИНОТЕХНИКА-АЛТАЙ"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ПРОИЗВОДСТВЕННО-КОММЕРЧЕСКАЯ ФИРМА "ДИЗЕЛЬ-АРСЕНАЛ"</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
         <is>
-          <t>г. Барнаул, Павловский тракт, д. 138, КВ.182</t>
+          <t>г. Ярославль, ул. Угличская, д. 39В, ОФИС 201</t>
         </is>
       </c>
       <c r="F11" s="7" t="inlineStr">
         <is>
-          <t>8 (3852) 22-26-48</t>
-        </is>
-      </c>
-      <c r="G11" s="7" t="inlineStr">
-        <is>
-          <t>biznes-region@mail.ru</t>
-        </is>
-      </c>
+          <t>8 (4852) 59-99-95</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr">
         <is>
-          <t>09.12.2013</t>
+          <t>28.09.2015</t>
         </is>
       </c>
       <c r="I11" s="7" t="inlineStr">
         <is>
-          <t>2222820223</t>
+          <t>7604286161</t>
         </is>
       </c>
       <c r="J11" s="7" t="inlineStr">
         <is>
-          <t>222201001</t>
+          <t>760401001</t>
         </is>
       </c>
       <c r="K11" s="7" t="inlineStr">
         <is>
-          <t>1132223015649</t>
+          <t>1157627021771</t>
         </is>
       </c>
       <c r="L11" s="7" t="inlineStr">
         <is>
-          <t>21441518</t>
+          <t>57758283</t>
         </is>
       </c>
       <c r="M11" s="7" t="inlineStr">
         <is>
-          <t>Солнцев Павел Николаевич</t>
+          <t>Головин Дмитрий Юрьевич</t>
         </is>
       </c>
       <c r="N11" s="7" t="inlineStr">
         <is>
-          <t>6.6 млн ₽</t>
+          <t>488.2 млн ₽</t>
         </is>
       </c>
       <c r="O11" s="7" t="inlineStr">
         <is>
-          <t>179 тыс ₽</t>
+          <t>604 тыс ₽</t>
         </is>
       </c>
       <c r="P11" s="7" t="inlineStr">
         <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="Q11" s="7" t="inlineStr">
+        <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="Q11" s="7" t="inlineStr">
+      <c r="R11" s="7" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="S11" s="7" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="R11" s="7" t="inlineStr">
+      <c r="T11" s="7" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="U11" s="7" t="inlineStr">
         <is>
           <t>100%</t>
         </is>
       </c>
-      <c r="S11" s="7" t="inlineStr"/>
-      <c r="T11" s="7" t="inlineStr"/>
-      <c r="U11" s="7" t="inlineStr"/>
       <c r="V11" s="7" t="inlineStr">
         <is>
-          <t>10 тыс ₽</t>
+          <t>1 млн ₽</t>
         </is>
       </c>
       <c r="W11" s="7" t="inlineStr">
         <is>
-          <t>1.1 млн ₽</t>
-        </is>
-      </c>
-      <c r="X11" s="7" t="inlineStr"/>
-      <c r="Y11" s="7" t="inlineStr"/>
-      <c r="Z11" s="7" t="inlineStr"/>
+          <t>22.8 млн ₽</t>
+        </is>
+      </c>
+      <c r="X11" s="7" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="Y11" s="7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="Z11" s="7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="AA11" s="7" t="inlineStr">
         <is>
-          <t>+ 70</t>
+          <t>+ 75</t>
         </is>
       </c>
       <c r="AB11" s="7" t="inlineStr">
         <is>
-          <t>- 1.9</t>
+          <t>- 7.6</t>
         </is>
       </c>
     </row>
@@ -2025,6 +2037,120 @@
         </is>
       </c>
       <c r="AB13" s="7" t="inlineStr">
+        <is>
+          <t>- 5.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>1.51</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>impuls-ek.ru</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>ТК "Импульс", ООО</t>
+        </is>
+      </c>
+      <c r="D14" s="7" t="inlineStr">
+        <is>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ ТОРГОВАЯ КОМПАНИЯ "ИМПУЛЬС"</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="inlineStr">
+        <is>
+          <t>г. Екатеринбург, ул. Расточная, д. 44, ПОМЕЩ. 104</t>
+        </is>
+      </c>
+      <c r="F14" s="7" t="inlineStr">
+        <is>
+          <t>8 (343) 217-63-09</t>
+        </is>
+      </c>
+      <c r="G14" s="7" t="inlineStr"/>
+      <c r="H14" s="7" t="inlineStr">
+        <is>
+          <t>13.09.2011</t>
+        </is>
+      </c>
+      <c r="I14" s="7" t="inlineStr">
+        <is>
+          <t>6670348122</t>
+        </is>
+      </c>
+      <c r="J14" s="7" t="inlineStr">
+        <is>
+          <t>667801001</t>
+        </is>
+      </c>
+      <c r="K14" s="7" t="inlineStr">
+        <is>
+          <t>1116670023491</t>
+        </is>
+      </c>
+      <c r="L14" s="7" t="inlineStr">
+        <is>
+          <t>30832301</t>
+        </is>
+      </c>
+      <c r="M14" s="7" t="inlineStr">
+        <is>
+          <t>Ушаков Александр Сергеевич</t>
+        </is>
+      </c>
+      <c r="N14" s="7" t="inlineStr">
+        <is>
+          <t>4.8 млн ₽</t>
+        </is>
+      </c>
+      <c r="O14" s="7" t="inlineStr">
+        <is>
+          <t>70 тыс ₽</t>
+        </is>
+      </c>
+      <c r="P14" s="7" t="inlineStr"/>
+      <c r="Q14" s="7" t="inlineStr"/>
+      <c r="R14" s="7" t="inlineStr"/>
+      <c r="S14" s="7" t="inlineStr"/>
+      <c r="T14" s="7" t="inlineStr"/>
+      <c r="U14" s="7" t="inlineStr"/>
+      <c r="V14" s="7" t="inlineStr">
+        <is>
+          <t>15 тыс ₽</t>
+        </is>
+      </c>
+      <c r="W14" s="7" t="inlineStr">
+        <is>
+          <t>2.1 млн ₽</t>
+        </is>
+      </c>
+      <c r="X14" s="7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Y14" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Z14" s="7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AA14" s="7" t="inlineStr">
+        <is>
+          <t>+ 66</t>
+        </is>
+      </c>
+      <c r="AB14" s="7" t="inlineStr">
         <is>
           <t>- 5.4</t>
         </is>
@@ -2450,212 +2576,208 @@
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
         <is>
-          <t>2.04</t>
+          <t>2.27</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>svarbi.ru</t>
+          <t>cin.ru</t>
         </is>
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Сварби, ООО</t>
+          <t>Фирма "ЦИН", ООО</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "СВАРБИ"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ФИРМА "ЦИН"</t>
         </is>
       </c>
       <c r="E5" s="7" t="inlineStr">
         <is>
-          <t>г. Москва, 1-й Дорожный проезд, д. 6, стр. 6</t>
-        </is>
-      </c>
-      <c r="F5" s="7" t="inlineStr"/>
+          <t>Московская обл., г. Люберцы, ул. Волковская, д. 69А</t>
+        </is>
+      </c>
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>8 (495) 774-69-43</t>
+        </is>
+      </c>
       <c r="G5" s="7" t="inlineStr">
         <is>
-          <t>info@svarbi.ru</t>
+          <t>mail@cin.ru</t>
         </is>
       </c>
       <c r="H5" s="7" t="inlineStr">
         <is>
-          <t>01.03.2001</t>
+          <t>11.08.1995</t>
         </is>
       </c>
       <c r="I5" s="7" t="inlineStr">
         <is>
-          <t>7726307154</t>
+          <t>5027011263</t>
         </is>
       </c>
       <c r="J5" s="7" t="inlineStr">
         <is>
-          <t>772601001</t>
+          <t>502701001</t>
         </is>
       </c>
       <c r="K5" s="7" t="inlineStr">
         <is>
-          <t>1027700015727</t>
+          <t>1025003209087</t>
         </is>
       </c>
       <c r="L5" s="7" t="inlineStr">
         <is>
-          <t>56521745</t>
+          <t>18037067</t>
         </is>
       </c>
       <c r="M5" s="7" t="inlineStr">
         <is>
-          <t>Тупицын Максим Витальевич</t>
+          <t>Елисеев Сергей Николаевич</t>
         </is>
       </c>
       <c r="N5" s="7" t="inlineStr">
         <is>
-          <t>773.6 млн ₽</t>
+          <t>6.4 млн ₽</t>
         </is>
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
-          <t>21.2 млн ₽</t>
-        </is>
-      </c>
-      <c r="P5" s="7" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
-      </c>
-      <c r="Q5" s="7" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="R5" s="7" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
-      </c>
+          <t>976 тыс ₽</t>
+        </is>
+      </c>
+      <c r="P5" s="7" t="inlineStr"/>
+      <c r="Q5" s="7" t="inlineStr"/>
+      <c r="R5" s="7" t="inlineStr"/>
       <c r="S5" s="7" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>43%</t>
         </is>
       </c>
       <c r="T5" s="7" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>28%</t>
         </is>
       </c>
       <c r="U5" s="7" t="inlineStr">
         <is>
-          <t>50%</t>
+          <t>29%</t>
         </is>
       </c>
       <c r="V5" s="7" t="inlineStr">
         <is>
-          <t>1 млн ₽</t>
+          <t>500 тыс ₽</t>
         </is>
       </c>
       <c r="W5" s="7" t="inlineStr">
         <is>
-          <t>100.6 млн ₽</t>
-        </is>
-      </c>
-      <c r="X5" s="7" t="inlineStr">
-        <is>
-          <t>756</t>
-        </is>
-      </c>
-      <c r="Y5" s="7" t="inlineStr">
-        <is>
-          <t>266</t>
-        </is>
-      </c>
-      <c r="Z5" s="7" t="inlineStr">
-        <is>
-          <t>159</t>
-        </is>
-      </c>
+          <t>56.4 млн ₽</t>
+        </is>
+      </c>
+      <c r="X5" s="7" t="inlineStr"/>
+      <c r="Y5" s="7" t="inlineStr"/>
+      <c r="Z5" s="7" t="inlineStr"/>
       <c r="AA5" s="7" t="inlineStr">
         <is>
-          <t>+ 82</t>
+          <t>+ 87</t>
         </is>
       </c>
       <c r="AB5" s="7" t="inlineStr">
         <is>
-          <t>- 4</t>
+          <t>- 2.2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>2.04</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>rezina-snab.ru</t>
+          <t>svarbi.ru</t>
         </is>
       </c>
       <c r="C6" s="7" t="inlineStr">
         <is>
-          <t>РТИ Экспресс, ООО</t>
+          <t>Сварби, ООО</t>
         </is>
       </c>
       <c r="D6" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "РТИ ЭКСПРЕСС"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "СВАРБИ"</t>
         </is>
       </c>
       <c r="E6" s="7" t="inlineStr">
         <is>
-          <t>г. Санкт-Петербург, ул. Зайцева, д. 41, лит. А, ПОМ. 15-Н;102</t>
+          <t>г. Москва, 1-й Дорожный проезд, д. 6, стр. 6</t>
         </is>
       </c>
       <c r="F6" s="7" t="inlineStr"/>
-      <c r="G6" s="7" t="inlineStr"/>
+      <c r="G6" s="7" t="inlineStr">
+        <is>
+          <t>info@svarbi.ru</t>
+        </is>
+      </c>
       <c r="H6" s="7" t="inlineStr">
         <is>
-          <t>22.12.2009</t>
+          <t>01.03.2001</t>
         </is>
       </c>
       <c r="I6" s="7" t="inlineStr">
         <is>
-          <t>7805508618</t>
+          <t>7726307154</t>
         </is>
       </c>
       <c r="J6" s="7" t="inlineStr">
         <is>
-          <t>780501001</t>
+          <t>772601001</t>
         </is>
       </c>
       <c r="K6" s="7" t="inlineStr">
         <is>
-          <t>1099847036816</t>
+          <t>1027700015727</t>
         </is>
       </c>
       <c r="L6" s="7" t="inlineStr">
         <is>
-          <t>64224642</t>
+          <t>56521745</t>
         </is>
       </c>
       <c r="M6" s="7" t="inlineStr">
         <is>
-          <t>Подгорный Кирилл Федорович</t>
+          <t>Тупицын Максим Витальевич</t>
         </is>
       </c>
       <c r="N6" s="7" t="inlineStr">
         <is>
-          <t>34.8 млн ₽</t>
+          <t>773.6 млн ₽</t>
         </is>
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
-          <t>4.4 млн ₽</t>
-        </is>
-      </c>
-      <c r="P6" s="7" t="inlineStr"/>
-      <c r="Q6" s="7" t="inlineStr"/>
-      <c r="R6" s="7" t="inlineStr"/>
+          <t>21.2 млн ₽</t>
+        </is>
+      </c>
+      <c r="P6" s="7" t="inlineStr">
+        <is>
+          <t>70%</t>
+        </is>
+      </c>
+      <c r="Q6" s="7" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="R6" s="7" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
       <c r="S6" s="7" t="inlineStr">
         <is>
           <t>50%</t>
@@ -2673,37 +2795,37 @@
       </c>
       <c r="V6" s="7" t="inlineStr">
         <is>
-          <t>10 тыс ₽</t>
+          <t>1 млн ₽</t>
         </is>
       </c>
       <c r="W6" s="7" t="inlineStr">
         <is>
-          <t>15.1 млн ₽</t>
+          <t>100.6 млн ₽</t>
         </is>
       </c>
       <c r="X6" s="7" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>761</t>
         </is>
       </c>
       <c r="Y6" s="7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>266</t>
         </is>
       </c>
       <c r="Z6" s="7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>159</t>
         </is>
       </c>
       <c r="AA6" s="7" t="inlineStr">
         <is>
-          <t>+ 79</t>
+          <t>+ 82</t>
         </is>
       </c>
       <c r="AB6" s="7" t="inlineStr">
         <is>
-          <t>- 1.2</t>
+          <t>- 4</t>
         </is>
       </c>
     </row>
@@ -2715,7 +2837,7 @@
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>rti-express.ru</t>
+          <t>rezina-snab.ru</t>
         </is>
       </c>
       <c r="C7" s="7" t="inlineStr">
@@ -2767,12 +2889,12 @@
       </c>
       <c r="N7" s="7" t="inlineStr">
         <is>
-          <t>34.8 млн ₽</t>
+          <t>45.4 млн ₽</t>
         </is>
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
-          <t>4.4 млн ₽</t>
+          <t>7.6 млн ₽</t>
         </is>
       </c>
       <c r="P7" s="7" t="inlineStr"/>
@@ -2800,7 +2922,7 @@
       </c>
       <c r="W7" s="7" t="inlineStr">
         <is>
-          <t>15.1 млн ₽</t>
+          <t>21.2 млн ₽</t>
         </is>
       </c>
       <c r="X7" s="7" t="inlineStr">
@@ -2832,97 +2954,89 @@
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
         <is>
-          <t>1.74</t>
+          <t>1.90</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>rizar.ru</t>
+          <t>rti-express.ru</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr">
         <is>
-          <t>Ризар, ООО</t>
+          <t>РТИ Экспресс, ООО</t>
         </is>
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "РИЗАР"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "РТИ ЭКСПРЕСС"</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>Волгоградская обл., г. Волжский, 1-й Индустриальный пр-д, Д.16, К.А</t>
-        </is>
-      </c>
-      <c r="F8" s="7" t="inlineStr">
-        <is>
-          <t>8 (8443) 24-01-17</t>
-        </is>
-      </c>
-      <c r="G8" s="7" t="inlineStr">
-        <is>
-          <t>rizar-rti@yandex.ru</t>
-        </is>
-      </c>
+          <t>г. Санкт-Петербург, ул. Зайцева, д. 41, лит. А, ПОМ. 15-Н;102</t>
+        </is>
+      </c>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>23.04.2013</t>
+          <t>22.12.2009</t>
         </is>
       </c>
       <c r="I8" s="7" t="inlineStr">
         <is>
-          <t>3435304715</t>
+          <t>7805508618</t>
         </is>
       </c>
       <c r="J8" s="7" t="inlineStr">
         <is>
-          <t>343501001</t>
+          <t>780501001</t>
         </is>
       </c>
       <c r="K8" s="7" t="inlineStr">
         <is>
-          <t>1133435002513</t>
+          <t>1099847036816</t>
         </is>
       </c>
       <c r="L8" s="7" t="inlineStr">
         <is>
-          <t>22353029</t>
+          <t>64224642</t>
         </is>
       </c>
       <c r="M8" s="7" t="inlineStr">
         <is>
-          <t>Тетерятникова Мария Сергеевна</t>
+          <t>Подгорный Кирилл Федорович</t>
         </is>
       </c>
       <c r="N8" s="7" t="inlineStr">
         <is>
-          <t>20.1 млн ₽</t>
+          <t>45.4 млн ₽</t>
         </is>
       </c>
       <c r="O8" s="7" t="inlineStr">
         <is>
-          <t>130 тыс ₽</t>
-        </is>
-      </c>
-      <c r="P8" s="7" t="inlineStr">
-        <is>
-          <t>80%</t>
-        </is>
-      </c>
-      <c r="Q8" s="7" t="inlineStr">
+          <t>7.6 млн ₽</t>
+        </is>
+      </c>
+      <c r="P8" s="7" t="inlineStr"/>
+      <c r="Q8" s="7" t="inlineStr"/>
+      <c r="R8" s="7" t="inlineStr"/>
+      <c r="S8" s="7" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="T8" s="7" t="inlineStr">
         <is>
           <t>0%</t>
         </is>
       </c>
-      <c r="R8" s="7" t="inlineStr">
-        <is>
-          <t>20%</t>
-        </is>
-      </c>
-      <c r="S8" s="7" t="inlineStr"/>
-      <c r="T8" s="7" t="inlineStr"/>
-      <c r="U8" s="7" t="inlineStr"/>
+      <c r="U8" s="7" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
       <c r="V8" s="7" t="inlineStr">
         <is>
           <t>10 тыс ₽</t>
@@ -2930,110 +3044,114 @@
       </c>
       <c r="W8" s="7" t="inlineStr">
         <is>
-          <t>4.7 млн ₽</t>
+          <t>21.2 млн ₽</t>
         </is>
       </c>
       <c r="X8" s="7" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>11</t>
         </is>
       </c>
       <c r="Y8" s="7" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>4</t>
         </is>
       </c>
       <c r="Z8" s="7" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AA8" s="7" t="inlineStr">
         <is>
-          <t>+ 78</t>
+          <t>+ 79</t>
         </is>
       </c>
       <c r="AB8" s="7" t="inlineStr">
         <is>
-          <t>- 5.4</t>
+          <t>- 1.2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
         <is>
-          <t>1.68</t>
+          <t>1.74</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>promresurs.ru</t>
+          <t>rizar.ru</t>
         </is>
       </c>
       <c r="C9" s="7" t="inlineStr">
         <is>
-          <t>Промресурссервис, ООО</t>
+          <t>Ризар, ООО</t>
         </is>
       </c>
       <c r="D9" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ПРОМРЕСУРССЕРВИС"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "РИЗАР"</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr">
         <is>
-          <t>Московская обл., г. Долгопрудный, ул. Зеленая, д. 1</t>
+          <t>Волгоградская обл., г. Волжский, 1-й Индустриальный пр-д, Д.16, К.А</t>
         </is>
       </c>
       <c r="F9" s="7" t="inlineStr">
         <is>
-          <t>8 (495) 526-68-26</t>
-        </is>
-      </c>
-      <c r="G9" s="7" t="inlineStr"/>
+          <t>8 (8443) 24-01-17</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr">
+        <is>
+          <t>rizar-rti@yandex.ru</t>
+        </is>
+      </c>
       <c r="H9" s="7" t="inlineStr">
         <is>
-          <t>11.12.2014</t>
+          <t>23.04.2013</t>
         </is>
       </c>
       <c r="I9" s="7" t="inlineStr">
         <is>
-          <t>5047162920</t>
+          <t>3435304715</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr">
         <is>
-          <t>504701001</t>
+          <t>343501001</t>
         </is>
       </c>
       <c r="K9" s="7" t="inlineStr">
         <is>
-          <t>1145047013363</t>
+          <t>1133435002513</t>
         </is>
       </c>
       <c r="L9" s="7" t="inlineStr">
         <is>
-          <t>39823025</t>
+          <t>22353029</t>
         </is>
       </c>
       <c r="M9" s="7" t="inlineStr">
         <is>
-          <t>Балакирев Виталий Владимирович</t>
+          <t>Тетерятникова Мария Сергеевна</t>
         </is>
       </c>
       <c r="N9" s="7" t="inlineStr">
         <is>
-          <t>317 млн ₽</t>
+          <t>20.1 млн ₽</t>
         </is>
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
-          <t>2.2 млн ₽</t>
+          <t>130 тыс ₽</t>
         </is>
       </c>
       <c r="P9" s="7" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="Q9" s="7" t="inlineStr">
@@ -3043,145 +3161,133 @@
       </c>
       <c r="R9" s="7" t="inlineStr">
         <is>
-          <t>27%</t>
-        </is>
-      </c>
-      <c r="S9" s="7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
-      <c r="T9" s="7" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="U9" s="7" t="inlineStr">
-        <is>
-          <t>0%</t>
-        </is>
-      </c>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="S9" s="7" t="inlineStr"/>
+      <c r="T9" s="7" t="inlineStr"/>
+      <c r="U9" s="7" t="inlineStr"/>
       <c r="V9" s="7" t="inlineStr">
         <is>
-          <t>100 тыс ₽</t>
+          <t>10 тыс ₽</t>
         </is>
       </c>
       <c r="W9" s="7" t="inlineStr">
         <is>
-          <t>30.5 млн ₽</t>
+          <t>4.7 млн ₽</t>
         </is>
       </c>
       <c r="X9" s="7" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>81</t>
         </is>
       </c>
       <c r="Y9" s="7" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>22</t>
         </is>
       </c>
       <c r="Z9" s="7" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>22</t>
         </is>
       </c>
       <c r="AA9" s="7" t="inlineStr">
         <is>
-          <t>+ 77</t>
+          <t>+ 78</t>
         </is>
       </c>
       <c r="AB9" s="7" t="inlineStr">
         <is>
-          <t>- 6.4</t>
+          <t>- 5.4</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
         <is>
-          <t>1.59</t>
+          <t>1.68</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>pulscen.ru</t>
+          <t>promresurs.ru</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr">
         <is>
-          <t>Издательство "ПУЛЬС Цен", ООО</t>
+          <t>Промресурссервис, ООО</t>
         </is>
       </c>
       <c r="D10" s="7" t="inlineStr">
         <is>
-          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ ИЗДАТЕЛЬСТВО "ПУЛЬС ЦЕН"</t>
+          <t>ОБЩЕСТВО С ОГРАНИЧЕННОЙ ОТВЕТСТВЕННОСТЬЮ "ПРОМРЕСУРССЕРВИС"</t>
         </is>
       </c>
       <c r="E10" s="7" t="inlineStr">
         <is>
-          <t>г. Екатеринбург, ул. Радищева, стр. 23, ОФИС 328/3</t>
+          <t>Московская обл., г. Долгопрудный, ул. Зеленая, д. 1</t>
         </is>
       </c>
       <c r="F10" s="7" t="inlineStr">
         <is>
-          <t>8 (343) 376-51-54</t>
+          <t>8 (495) 526-68-26</t>
         </is>
       </c>
       <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr">
         <is>
-          <t>09.12.1999</t>
+          <t>11.12.2014</t>
         </is>
       </c>
       <c r="I10" s="7" t="inlineStr">
         <is>
-          <t>6664071183</t>
+          <t>5047162920</t>
         </is>
       </c>
       <c r="J10" s="7" t="inlineStr">
         <is>
-          <t>667101001</t>
+          <t>504701001</t>
         </is>
       </c>
       <c r="K10" s="7" t="inlineStr">
         <is>
-          <t>1026605758442</t>
+          <t>1145047013363</t>
         </is>
       </c>
       <c r="L10" s="7" t="inlineStr">
         <is>
-          <t>52319372</t>
+          <t>39823025</t>
         </is>
       </c>
       <c r="M10" s="7" t="inlineStr">
         <is>
-          <t>Харитонов Алексей Владимирович</t>
+          <t>Балакирев Виталий Владимирович</t>
         </is>
       </c>
       <c r="N10" s="7" t="inlineStr">
         <is>
-          <t>1.9 млн ₽</t>
+          <t>317 млн ₽</t>
         </is>
       </c>
       <c r="O10" s="7" t="inlineStr">
         <is>
-          <t>-2.2 млн ₽</t>
+          <t>2.2 млн ₽</t>
         </is>
       </c>
       <c r="P10" s="7" t="inlineStr">
         <is>
-          <t>18%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="Q10" s="7" t="inlineStr">
         <is>
-          <t>6%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="R10" s="7" t="inlineStr">
         <is>
-          <t>76%</t>
+          <t>27%</t>
         </is>
       </c>
       <c r="S10" s="7" t="inlineStr">
@@ -3191,35 +3297,47 @@
       </c>
       <c r="T10" s="7" t="inlineStr">
         <is>
-          <t>9%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="U10" s="7" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>0%</t>
         </is>
       </c>
       <c r="V10" s="7" t="inlineStr">
         <is>
-          <t>10 тыс ₽</t>
+          <t>100 тыс ₽</t>
         </is>
       </c>
       <c r="W10" s="7" t="inlineStr">
         <is>
-          <t>2.9 млн ₽</t>
-        </is>
-      </c>
-      <c r="X10" s="7" t="inlineStr"/>
-      <c r="Y10" s="7" t="inlineStr"/>
-      <c r="Z10" s="7" t="inlineStr"/>
+          <t>30.5 млн ₽</t>
+        </is>
+      </c>
+      <c r="X10" s="7" t="inlineStr">
+        <is>
+          <t>267</t>
+        </is>
+      </c>
+      <c r="Y10" s="7" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="Z10" s="7" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
       <c r="AA10" s="7" t="inlineStr">
         <is>
-          <t>+ 65</t>
+          <t>+ 77</t>
         </is>
       </c>
       <c r="AB10" s="7" t="inlineStr">
         <is>
-          <t>- 7.7</t>
+          <t>- 6.4</t>
         </is>
       </c>
     </row>

</xml_diff>